<commit_message>
add goong io map api for coordinate,clusters map
</commit_message>
<xml_diff>
--- a/DASA1.xlsx
+++ b/DASA1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Hoc\Projects\hethongthongminh\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB468E3E-88CE-470D-B4F8-0AC8F6CAC4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4A22CC-ADD5-48CE-8AB5-F7CEEFCD0D75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="327">
   <si>
     <t>Địa chỉ nhà</t>
   </si>
@@ -210,9 +210,6 @@
     <t>Võ Thị Hương</t>
   </si>
   <si>
-    <t>32 Nguyễn Văn Linh, phường Vĩnh Trung</t>
-  </si>
-  <si>
     <t>Lê Thị Mai</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Phạm Thị Hoa</t>
   </si>
   <si>
-    <t>11 Tô Ngọc Vân, phường Linh Tây</t>
-  </si>
-  <si>
     <t>Trần Minh Hải</t>
   </si>
   <si>
@@ -975,12 +969,6 @@
     <t>20.997468935118016</t>
   </si>
   <si>
-    <t>20.060499</t>
-  </si>
-  <si>
-    <t>21.0747580</t>
-  </si>
-  <si>
     <t>21.0131391</t>
   </si>
   <si>
@@ -1000,6 +988,24 @@
   </si>
   <si>
     <t>12 Lê Hồng Phong</t>
+  </si>
+  <si>
+    <t>105.82527436822804</t>
+  </si>
+  <si>
+    <t>21.068137741691334</t>
+  </si>
+  <si>
+    <t>11 Tô Ngọc Vân</t>
+  </si>
+  <si>
+    <t>21.03635774477897</t>
+  </si>
+  <si>
+    <t>105.79001216969687</t>
+  </si>
+  <si>
+    <t>334 Cầu Giấy</t>
   </si>
 </sst>
 </file>
@@ -1368,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,8 +1383,8 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.7109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1387,15 +1393,15 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1"/>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1410,11 +1416,11 @@
       <c r="C2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="2">
         <v>105.81032244281</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="F2" s="2">
         <v>4.4000000000000004</v>
@@ -1430,11 +1436,11 @@
       <c r="C3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="2">
         <v>105.806701408824</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="F3" s="2">
         <v>4.8</v>
@@ -1450,11 +1456,11 @@
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="2">
         <v>105.82230587855599</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="F4" s="2">
         <v>3.2</v>
@@ -1470,11 +1476,11 @@
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="2">
         <v>105.791127076644</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="F5" s="2">
         <v>6.8</v>
@@ -1490,11 +1496,11 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="2">
         <v>105.795255224729</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="F6" s="2">
         <v>5.7</v>
@@ -1510,11 +1516,11 @@
       <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="2">
         <v>105.844420055303</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="F7" s="2">
         <v>2.5</v>
@@ -1530,11 +1536,11 @@
       <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="2">
         <v>105.81292728867901</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="F8" s="2">
         <v>3.6</v>
@@ -1550,11 +1556,11 @@
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="2">
         <v>105.827454503227</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="F9" s="2">
         <v>5.2</v>
@@ -1570,11 +1576,11 @@
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="2">
         <v>105.801562186119</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="F10" s="2">
         <v>3.9</v>
@@ -1590,11 +1596,11 @@
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D11" s="2">
         <v>105.8141240628</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="F11" s="2">
         <v>4.3</v>
@@ -1610,11 +1616,11 @@
       <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="2">
         <v>105.81284346299999</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="F12" s="2">
         <v>3.9</v>
@@ -1630,11 +1636,11 @@
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="2">
         <v>105.80291017010001</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="F13" s="2">
         <v>5.9</v>
@@ -1650,11 +1656,11 @@
       <c r="C14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="2">
         <v>105.843757166</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>224</v>
       </c>
       <c r="F14" s="2">
         <v>4.0999999999999996</v>
@@ -1670,11 +1676,11 @@
       <c r="C15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="D15" s="2">
         <v>105.85625295299999</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>225</v>
       </c>
       <c r="F15" s="2">
         <v>3.2</v>
@@ -1690,11 +1696,11 @@
       <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="2">
         <v>105.81500733</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>226</v>
       </c>
       <c r="F16" s="2">
         <v>5.2</v>
@@ -1710,11 +1716,11 @@
       <c r="C17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="2">
         <v>105.7873040835</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>227</v>
       </c>
       <c r="F17" s="2">
         <v>5.6</v>
@@ -1730,11 +1736,11 @@
       <c r="C18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D18" s="2">
         <v>105.81251213</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>228</v>
       </c>
       <c r="F18" s="2">
         <v>4.4000000000000004</v>
@@ -1750,11 +1756,11 @@
       <c r="C19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="2">
         <v>105.811295704</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="F19" s="2">
         <v>4.8</v>
@@ -1770,11 +1776,11 @@
       <c r="C20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="2">
         <v>105.793096151</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="F20" s="2">
         <v>5.5</v>
@@ -1790,11 +1796,11 @@
       <c r="C21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D21" s="3">
         <v>105.851051968269</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>231</v>
       </c>
       <c r="F21" s="3">
         <v>1.92</v>
@@ -1810,11 +1816,11 @@
       <c r="C22" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="D22" s="3">
         <v>105.80130106854</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>232</v>
       </c>
       <c r="F22" s="3">
         <v>4.38</v>
@@ -1830,11 +1836,11 @@
       <c r="C23" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="E23" s="3">
+      <c r="D23" s="3">
         <v>105.812151394309</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>233</v>
       </c>
       <c r="F23" s="3">
         <v>3.09</v>
@@ -1850,11 +1856,11 @@
       <c r="C24" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="E24" s="3">
+      <c r="D24" s="3">
         <v>105.84714346008001</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>234</v>
       </c>
       <c r="F24" s="3">
         <v>2.38</v>
@@ -1870,11 +1876,11 @@
       <c r="C25" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="D25" s="3">
         <v>105.787732017547</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="F25" s="3">
         <v>5.03</v>
@@ -1890,11 +1896,11 @@
       <c r="C26" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="E26" s="3">
+      <c r="D26" s="3">
         <v>105.857375507832</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>236</v>
       </c>
       <c r="F26" s="3">
         <v>2.4700000000000002</v>
@@ -1910,11 +1916,11 @@
       <c r="C27" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E27" s="3">
+      <c r="D27" s="3">
         <v>105.793809016759</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>237</v>
       </c>
       <c r="F27" s="3">
         <v>4.63</v>
@@ -1930,11 +1936,11 @@
       <c r="C28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="D28" s="3">
         <v>105.85037343716201</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>238</v>
       </c>
       <c r="F28" s="3">
         <v>2.97</v>
@@ -1950,11 +1956,11 @@
       <c r="C29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="E29" s="3">
+      <c r="D29" s="3">
         <v>105.802778452292</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>239</v>
       </c>
       <c r="F29" s="3">
         <v>3.87</v>
@@ -1967,14 +1973,14 @@
       <c r="B30" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>61</v>
+      <c r="C30" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="E30" s="3">
-        <v>108.216159</v>
+        <v>325</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>324</v>
       </c>
       <c r="F30" s="3">
         <v>2.6</v>
@@ -1985,16 +1991,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="D31" s="3">
         <v>105.81275100000001</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>240</v>
       </c>
       <c r="F31" s="3">
         <v>3.6</v>
@@ -2005,16 +2011,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F32" s="3">
         <v>4.9000000000000004</v>
@@ -2025,16 +2031,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="E33" s="3">
+      <c r="D33" s="3">
         <v>105.80996</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>241</v>
       </c>
       <c r="F33" s="3">
         <v>3.8</v>
@@ -2045,16 +2051,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>323</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="E34" s="3">
-        <v>106.65069</v>
+        <v>321</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>322</v>
       </c>
       <c r="F34" s="3">
         <v>5.8</v>
@@ -2065,16 +2071,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F35" s="3">
         <v>4.4000000000000004</v>
@@ -2085,16 +2091,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="E36" s="3">
+        <v>70</v>
+      </c>
+      <c r="D36" s="3">
         <v>105.824139</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>242</v>
       </c>
       <c r="F36" s="3">
         <v>3.9</v>
@@ -2105,16 +2111,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F37" s="3">
         <v>5</v>
@@ -2125,16 +2131,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="E38" s="3">
+        <v>74</v>
+      </c>
+      <c r="D38" s="3">
         <v>105.85419</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>243</v>
       </c>
       <c r="F38" s="3">
         <v>3.3</v>
@@ -2145,16 +2151,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E39" s="3">
+        <v>76</v>
+      </c>
+      <c r="D39" s="3">
         <v>105.849686930461</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>244</v>
       </c>
       <c r="F39" s="3">
         <v>1.74</v>
@@ -2165,16 +2171,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>247</v>
-      </c>
-      <c r="E40" s="3">
+        <v>78</v>
+      </c>
+      <c r="D40" s="3">
         <v>105.818744647651</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>245</v>
       </c>
       <c r="F40" s="3">
         <v>4.37</v>
@@ -2185,16 +2191,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="E41" s="3">
+        <v>80</v>
+      </c>
+      <c r="D41" s="3">
         <v>105.813811137371</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="F41" s="3">
         <v>3.33</v>
@@ -2205,16 +2211,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="E42" s="3">
+        <v>82</v>
+      </c>
+      <c r="D42" s="3">
         <v>105.892694311203</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>247</v>
       </c>
       <c r="F42" s="3">
         <v>4.8499999999999996</v>
@@ -2225,16 +2231,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E43" s="3">
+        <v>84</v>
+      </c>
+      <c r="D43" s="3">
         <v>105.848099237657</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>248</v>
       </c>
       <c r="F43" s="3">
         <v>1.52</v>
@@ -2245,16 +2251,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="E44" s="3">
+        <v>86</v>
+      </c>
+      <c r="D44" s="3">
         <v>105.849119363746</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>249</v>
       </c>
       <c r="F44" s="3">
         <v>1.43</v>
@@ -2265,16 +2271,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="E45" s="3">
+        <v>88</v>
+      </c>
+      <c r="D45" s="3">
         <v>105.847802313299</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>250</v>
       </c>
       <c r="F45" s="3">
         <v>2.35</v>
@@ -2285,16 +2291,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E46" s="3">
+        <v>90</v>
+      </c>
+      <c r="D46" s="3">
         <v>105.790475064879</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="F46" s="3">
         <v>5.3</v>
@@ -2305,16 +2311,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="E47" s="3">
+        <v>92</v>
+      </c>
+      <c r="D47" s="3">
         <v>105.852290974317</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="F47" s="3">
         <v>2.98</v>
@@ -2325,16 +2331,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="E48" s="3">
+        <v>95</v>
+      </c>
+      <c r="D48" s="3">
         <v>105.86583160000001</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>253</v>
       </c>
       <c r="F48" s="3">
         <v>5.16</v>
@@ -2345,16 +2351,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="E49" s="3">
+        <v>97</v>
+      </c>
+      <c r="D49" s="3">
         <v>105.7621843</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>254</v>
       </c>
       <c r="F49" s="3">
         <v>5.96</v>
@@ -2365,16 +2371,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="E50" s="3">
+        <v>99</v>
+      </c>
+      <c r="D50" s="3">
         <v>105.81085109999999</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>255</v>
       </c>
       <c r="F50" s="3">
         <v>4.4800000000000004</v>
@@ -2385,16 +2391,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="E51" s="3">
+        <v>101</v>
+      </c>
+      <c r="D51" s="3">
         <v>105.82121069999999</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>256</v>
       </c>
       <c r="F51" s="3">
         <v>4</v>
@@ -2405,16 +2411,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="E52" s="3">
+        <v>103</v>
+      </c>
+      <c r="D52" s="3">
         <v>105.7992653</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>257</v>
       </c>
       <c r="F52" s="3">
         <v>3.85</v>
@@ -2425,16 +2431,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="E53" s="3">
+        <v>105</v>
+      </c>
+      <c r="D53" s="3">
         <v>105.85999440000001</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>258</v>
       </c>
       <c r="F53" s="3">
         <v>5.6</v>
@@ -2445,16 +2451,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="E54" s="3">
+        <v>107</v>
+      </c>
+      <c r="D54" s="3">
         <v>105.8179761</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>259</v>
       </c>
       <c r="F54" s="3">
         <v>5.56</v>
@@ -2465,16 +2471,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="E55" s="3">
+        <v>109</v>
+      </c>
+      <c r="D55" s="3">
         <v>105.8117402</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>260</v>
       </c>
       <c r="F55" s="3">
         <v>4.4800000000000004</v>
@@ -2485,16 +2491,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="E56" s="3">
+        <v>111</v>
+      </c>
+      <c r="D56" s="3">
         <v>105.8027965</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>261</v>
       </c>
       <c r="F56" s="3">
         <v>5.39</v>
@@ -2505,16 +2511,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="E57" s="3">
+        <v>113</v>
+      </c>
+      <c r="D57" s="3">
         <v>105.8442336</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="F57" s="3">
         <v>5.25</v>
@@ -2525,16 +2531,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="E58" s="4">
+        <v>115</v>
+      </c>
+      <c r="D58" s="4">
         <v>105.78703394588101</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>263</v>
       </c>
       <c r="F58" s="4">
         <v>6.3</v>
@@ -2545,16 +2551,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E59" s="4">
+        <v>117</v>
+      </c>
+      <c r="D59" s="4">
         <v>105.80803993377199</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>264</v>
       </c>
       <c r="F59" s="4">
         <v>3.7</v>
@@ -2565,16 +2571,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E60" s="4">
+        <v>119</v>
+      </c>
+      <c r="D60" s="4">
         <v>105.816200300145</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>265</v>
       </c>
       <c r="F60" s="4">
         <v>4.5</v>
@@ -2585,16 +2591,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="E61" s="4">
+        <v>121</v>
+      </c>
+      <c r="D61" s="4">
         <v>105.78847887002</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>266</v>
       </c>
       <c r="F61" s="4">
         <v>6.9</v>
@@ -2605,16 +2611,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D62" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="E62" s="4">
+        <v>123</v>
+      </c>
+      <c r="D62" s="4">
         <v>105.803247824377</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>267</v>
       </c>
       <c r="F62" s="4">
         <v>4.8</v>
@@ -2625,16 +2631,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="D63" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="E63" s="4">
+        <v>125</v>
+      </c>
+      <c r="D63" s="4">
         <v>105.822116184181</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>268</v>
       </c>
       <c r="F63" s="4">
         <v>5.6</v>
@@ -2645,16 +2651,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="E64" s="4">
+        <v>141</v>
+      </c>
+      <c r="D64" s="4">
         <v>105.811221768447</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>269</v>
       </c>
       <c r="F64" s="4">
         <v>3.3</v>
@@ -2665,16 +2671,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D65" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="E65" s="4">
+        <v>143</v>
+      </c>
+      <c r="D65" s="4">
         <v>105.808473487496</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>270</v>
       </c>
       <c r="F65" s="4">
         <v>6.4</v>
@@ -2685,16 +2691,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="E66" s="4">
+        <v>144</v>
+      </c>
+      <c r="D66" s="4">
         <v>105.811809207352</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>271</v>
       </c>
       <c r="F66" s="4">
         <v>3.6</v>
@@ -2705,16 +2711,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E67" s="4">
+        <v>146</v>
+      </c>
+      <c r="D67" s="4">
         <v>105.810480154391</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>272</v>
       </c>
       <c r="F67" s="4">
         <v>6.4</v>
@@ -2725,16 +2731,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D68" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="E68" s="4">
+        <v>129</v>
+      </c>
+      <c r="D68" s="4">
         <v>105.80932258562299</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>273</v>
       </c>
       <c r="F68" s="4">
         <v>5.0999999999999996</v>
@@ -2745,16 +2751,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="E69" s="4">
+        <v>130</v>
+      </c>
+      <c r="D69" s="4">
         <v>105.81805630241401</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="F69" s="4">
         <v>4.5999999999999996</v>
@@ -2765,16 +2771,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="D70" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="E70" s="4">
+        <v>132</v>
+      </c>
+      <c r="D70" s="4">
         <v>105.802664259342</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="F70" s="4">
         <v>5.5</v>
@@ -2785,16 +2791,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="E71" s="4">
+        <v>134</v>
+      </c>
+      <c r="D71" s="4">
         <v>105.80950696247901</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>276</v>
       </c>
       <c r="F71" s="4">
         <v>3.5</v>
@@ -2805,16 +2811,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="E72" s="4">
+        <v>136</v>
+      </c>
+      <c r="D72" s="4">
         <v>105.803326413617</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>277</v>
       </c>
       <c r="F72" s="4">
         <v>6.8</v>
@@ -2825,16 +2831,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="E73" s="4">
+        <v>138</v>
+      </c>
+      <c r="D73" s="4">
         <v>105.79587469282301</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>278</v>
       </c>
       <c r="F73" s="4">
         <v>6.1</v>
@@ -2845,16 +2851,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D74" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="E74" s="4">
+        <v>139</v>
+      </c>
+      <c r="D74" s="4">
         <v>105.827717039156</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>279</v>
       </c>
       <c r="F74" s="4">
         <v>6.7</v>
@@ -2865,16 +2871,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="E75" s="4">
+        <v>148</v>
+      </c>
+      <c r="D75" s="4">
         <v>105.80992500000001</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>280</v>
       </c>
       <c r="F75" s="4">
         <v>4.3</v>
@@ -2885,16 +2891,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="E76" s="4">
+        <v>150</v>
+      </c>
+      <c r="D76" s="4">
         <v>105.81022</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>281</v>
       </c>
       <c r="F76" s="4">
         <v>3.5</v>
@@ -2908,13 +2914,13 @@
         <v>6</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E77" s="4">
+        <v>151</v>
+      </c>
+      <c r="D77" s="4">
         <v>105.8035575</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>282</v>
       </c>
       <c r="F77" s="4">
         <v>4.3</v>
@@ -2925,16 +2931,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="E78" s="4">
+        <v>153</v>
+      </c>
+      <c r="D78" s="4">
         <v>105.8093612</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>283</v>
       </c>
       <c r="F78" s="4">
         <v>4.7</v>
@@ -2945,16 +2951,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D79" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="E79" s="4">
+        <v>155</v>
+      </c>
+      <c r="D79" s="4">
         <v>105.8122858</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>284</v>
       </c>
       <c r="F79" s="4">
         <v>5.6</v>
@@ -2965,16 +2971,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="E80" s="4">
+        <v>157</v>
+      </c>
+      <c r="D80" s="4">
         <v>105.811644197418</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>285</v>
       </c>
       <c r="F80" s="4">
         <v>5.0999999999999996</v>
@@ -2985,16 +2991,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="D81" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="E81" s="4">
+        <v>159</v>
+      </c>
+      <c r="D81" s="4">
         <v>105.80706771439</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>286</v>
       </c>
       <c r="F81" s="4">
         <v>4.7</v>
@@ -3005,16 +3011,16 @@
         <v>81</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="E82" s="4">
+        <v>161</v>
+      </c>
+      <c r="D82" s="4">
         <v>105.81701360561</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>287</v>
       </c>
       <c r="F82" s="4">
         <v>6.8</v>
@@ -3025,16 +3031,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="E83" s="4">
+        <v>163</v>
+      </c>
+      <c r="D83" s="4">
         <v>105.80985304087901</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="F83" s="4">
         <v>3.3</v>
@@ -3045,16 +3051,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D84" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="E84" s="4">
+        <v>165</v>
+      </c>
+      <c r="D84" s="4">
         <v>105.849008716261</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>289</v>
       </c>
       <c r="F84" s="4">
         <v>4.4000000000000004</v>
@@ -3065,16 +3071,16 @@
         <v>84</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="E85" s="4">
+        <v>167</v>
+      </c>
+      <c r="D85" s="4">
         <v>105.83297654845801</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>290</v>
       </c>
       <c r="F85" s="4">
         <v>3.6</v>
@@ -3085,16 +3091,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D86" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="E86" s="4">
+        <v>168</v>
+      </c>
+      <c r="D86" s="4">
         <v>105.80913003833101</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>291</v>
       </c>
       <c r="F86" s="4">
         <v>3.5</v>
@@ -3105,16 +3111,16 @@
         <v>86</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="E87" s="4">
+        <v>170</v>
+      </c>
+      <c r="D87" s="4">
         <v>105.836375033243</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>292</v>
       </c>
       <c r="F87" s="4">
         <v>3.7</v>
@@ -3125,16 +3131,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D88" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="E88" s="4">
+        <v>172</v>
+      </c>
+      <c r="D88" s="4">
         <v>105.832986166764</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>293</v>
       </c>
       <c r="F88" s="4">
         <v>3.5</v>
@@ -3145,16 +3151,16 @@
         <v>88</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="E89" s="4">
+        <v>174</v>
+      </c>
+      <c r="D89" s="4">
         <v>105.814497305107</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>294</v>
       </c>
       <c r="F89" s="4">
         <v>3.3</v>
@@ -3165,16 +3171,16 @@
         <v>89</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D90" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="E90" s="4">
+        <v>176</v>
+      </c>
+      <c r="D90" s="4">
         <v>105.81835711748199</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>295</v>
       </c>
       <c r="F90" s="4">
         <v>3.3</v>
@@ -3185,16 +3191,16 @@
         <v>90</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="D91" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="E91" s="4">
+        <v>178</v>
+      </c>
+      <c r="D91" s="4">
         <v>105.820758039263</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>296</v>
       </c>
       <c r="F91" s="4">
         <v>3.5</v>
@@ -3205,16 +3211,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="E92" s="4">
+        <v>180</v>
+      </c>
+      <c r="D92" s="4">
         <v>105.810478997798</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>297</v>
       </c>
       <c r="F92" s="4">
         <v>3.6</v>
@@ -3225,16 +3231,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="E93" s="4">
+        <v>182</v>
+      </c>
+      <c r="D93" s="4">
         <v>105.774787450121</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>298</v>
       </c>
       <c r="F93" s="4">
         <v>4.7</v>
@@ -3245,16 +3251,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="E94" s="4">
+        <v>184</v>
+      </c>
+      <c r="D94" s="4">
         <v>105.84809821475</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="F94" s="4">
         <v>4.8</v>
@@ -3265,16 +3271,16 @@
         <v>94</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="E95" s="4">
+        <v>186</v>
+      </c>
+      <c r="D95" s="4">
         <v>105.819603259757</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>300</v>
       </c>
       <c r="F95" s="4">
         <v>4.3</v>
@@ -3285,16 +3291,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="E96" s="4">
+        <v>188</v>
+      </c>
+      <c r="D96" s="4">
         <v>105.813526465217</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>301</v>
       </c>
       <c r="F96" s="4">
         <v>3.8</v>
@@ -3305,16 +3311,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D97" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="E97" s="4">
+        <v>190</v>
+      </c>
+      <c r="D97" s="4">
         <v>105.85180084429101</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>302</v>
       </c>
       <c r="F97" s="4">
         <v>4.9000000000000004</v>
@@ -3325,16 +3331,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D98" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="E98" s="4">
+        <v>192</v>
+      </c>
+      <c r="D98" s="4">
         <v>105.81096313514099</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="F98" s="4">
         <v>4.5999999999999996</v>
@@ -3345,16 +3351,16 @@
         <v>98</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="D99" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="E99" s="4">
+        <v>194</v>
+      </c>
+      <c r="D99" s="4">
         <v>105.79330212237301</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>304</v>
       </c>
       <c r="F99" s="4">
         <v>4.9000000000000004</v>
@@ -3365,16 +3371,16 @@
         <v>99</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D100" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="E100" s="4">
+        <v>196</v>
+      </c>
+      <c r="D100" s="4">
         <v>105.812697613401</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="F100" s="4">
         <v>4.2</v>
@@ -3385,16 +3391,16 @@
         <v>100</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="D101" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="E101" s="4">
+        <v>198</v>
+      </c>
+      <c r="D101" s="4">
         <v>105.811568303654</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="F101" s="4">
         <v>4.7</v>
@@ -3405,16 +3411,16 @@
         <v>101</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>309</v>
-      </c>
-      <c r="E102" s="4">
+        <v>200</v>
+      </c>
+      <c r="D102" s="4">
         <v>105.801572527658</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>307</v>
       </c>
       <c r="F102" s="4">
         <v>4.9000000000000004</v>
@@ -3425,16 +3431,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="E103" s="4">
+        <v>202</v>
+      </c>
+      <c r="D103" s="4">
         <v>105.819570582168</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>308</v>
       </c>
       <c r="F103" s="4">
         <v>4.8</v>
@@ -3445,16 +3451,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="E104" s="4">
+        <v>203</v>
+      </c>
+      <c r="D104" s="4">
         <v>105.808902401029</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>309</v>
       </c>
       <c r="F104" s="4">
         <v>4.4000000000000004</v>
@@ -3465,16 +3471,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D105" s="4" t="s">
-        <v>312</v>
-      </c>
-      <c r="E105" s="4">
+        <v>205</v>
+      </c>
+      <c r="D105" s="4">
         <v>105.812938396877</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>310</v>
       </c>
       <c r="F105" s="4">
         <v>4.2</v>
@@ -3485,16 +3491,16 @@
         <v>105</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="E106" s="4">
+        <v>207</v>
+      </c>
+      <c r="D106" s="4">
         <v>105.81627215501</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="F106" s="4">
         <v>4.5</v>
@@ -3505,16 +3511,16 @@
         <v>106</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D107" s="4" t="s">
-        <v>314</v>
-      </c>
-      <c r="E107" s="4">
+        <v>209</v>
+      </c>
+      <c r="D107" s="4">
         <v>105.812678561007</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="F107" s="4">
         <v>4.2</v>
@@ -3525,16 +3531,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D108" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="E108" s="4">
+        <v>211</v>
+      </c>
+      <c r="D108" s="4">
         <v>105.80570787069701</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="F108" s="4">
         <v>4.9000000000000004</v>

</xml_diff>